<commit_message>
Updated bus error vplan from review feedback
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/Simulation/bus_error/CV32E40X_VerifPlan_Bus_Error.xlsx
+++ b/docs/VerifPlans/Simulation/bus_error/CV32E40X_VerifPlan_Bus_Error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\localWork\openHW\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F03383-718A-4686-AFE1-9B6ABAE8DA82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102DBF99-46C3-4B7E-8A8B-302E68F5E462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="121">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -118,15 +118,6 @@
   </si>
   <si>
     <t>Git Hub Hash (if appropriate)</t>
-  </si>
-  <si>
-    <t>OBIv1.0</t>
-  </si>
-  <si>
-    <t>Open Bus Interface (OBI) Specification, v1.0, 3/5/2020</t>
-  </si>
-  <si>
-    <t>https://github.com/openhwgroup/core-v-docs/blob/master/cores/cv32e40p/OBI-v1.0.pdf</t>
   </si>
   <si>
     <t>OBI compliance</t>
@@ -139,19 +130,10 @@
     <t xml:space="preserve">The OBI spec defines a bus error signal (err) that incidates the returning rdata field is invalid. </t>
   </si>
   <si>
-    <t>Verify that the bus error signal complies with OBI specification</t>
-  </si>
-  <si>
-    <t>2fe7db275f1c0a28e6093e60db503cd273e30080</t>
-  </si>
-  <si>
     <t>https://github.com/openhwgroup/cv32e40x/blob/master/docs/user_manual</t>
   </si>
   <si>
     <t>CV32E40X User Manual</t>
-  </si>
-  <si>
-    <t>UM 2fe7db</t>
   </si>
   <si>
     <t>A bus error on an instruction that does not get executed is ignored</t>
@@ -281,34 +263,6 @@
     </r>
   </si>
   <si>
-    <t>Instruction bus error priority</t>
-  </si>
-  <si>
-    <t>Verify that the bus error interrupts has the correct priority</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The priority of an instruction bus error is defined in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t>Interrupts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t xml:space="preserve"> section of the CV32E40X User Manual</t>
-    </r>
-  </si>
-  <si>
     <t>Misaligned instructions</t>
   </si>
   <si>
@@ -318,13 +272,7 @@
     <t>Partial instruction bus error</t>
   </si>
   <si>
-    <t>Verify that an instruction that is only partially contained in a faulty bus transaction causes an exception</t>
-  </si>
-  <si>
     <t>Shared instruction bus error</t>
-  </si>
-  <si>
-    <t>Verify that a compressed instruction that shares the bus transaction with another instruction causes an exception</t>
   </si>
   <si>
     <t>non-maskable when single-stepping</t>
@@ -493,53 +441,268 @@
     <t>Missing/required features</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The OBI agent will be required to randomly generate bus errors, and verify that the signals </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t xml:space="preserve">instr_err_i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t>data_err_i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t xml:space="preserve"> comply with the OBI Spec. </t>
-    </r>
-  </si>
-  <si>
     <t>UVM Scoreboard</t>
-  </si>
-  <si>
-    <t>Instruction set simulators need to be notified and take in to account instruction bus errors, and predict how the core will react to the resulting precise exception. This capability will be necessary in order to fully verify bus error operation on the core.</t>
   </si>
   <si>
     <t>As data bus errors does not result in a precise exception, but rather an NMI, these are not fit for prediction in the instruction set simulators. Therefore the scoreboard must be expanded to take these in to account, and verify that the interrupt appears within reasonable time, and are handled according to spec.
 Pass/fail criteria marked as "other" in this plan is intended to be checked by the scoreboard.</t>
+  </si>
+  <si>
+    <t>Instruction set simulators need to be notified and take in to account instruction bus errors, and predict how the core will react to the resulting precise exception. This capability will be necessary in order to fully verify instruction bus error operation on the core.</t>
+  </si>
+  <si>
+    <t>cover point of feature</t>
+  </si>
+  <si>
+    <t>Instruction group vs bus error cover point</t>
+  </si>
+  <si>
+    <t>828dac80e6ef2868d1ed9be0d78448ea93f4cddf</t>
+  </si>
+  <si>
+    <t>UM 828dac</t>
+  </si>
+  <si>
+    <t>Shall be specified in separate OBI verification plan</t>
+  </si>
+  <si>
+    <t>https://github.com/openhwgroup/core-v-docs/blob/master/cores/obi/OBI-v1.2.pdf</t>
+  </si>
+  <si>
+    <t>OBIv1.2</t>
+  </si>
+  <si>
+    <t>Open Bus Interface (OBI) Specification, v1.2, 4/15/2021</t>
+  </si>
+  <si>
+    <t>Debug interaction of instruction bus error</t>
+  </si>
+  <si>
+    <t>Instruction bus error while in debug</t>
+  </si>
+  <si>
+    <t>Instruction bus error while single stepping</t>
+  </si>
+  <si>
+    <t>Verify value of nmip bit of dcsr</t>
+  </si>
+  <si>
+    <t>Verify that an instruction that is only partially contained in a faulty bus transaction causes an exception
+Specific checks required:
+Error on word aligned 32-bit instruction.
+Error on lower half of non-word aligned 32-bit instruction.
+Error on upper half of non-word aligned 32-bit instruction.</t>
+  </si>
+  <si>
+    <t>Verify that a compressed instruction that shares the bus transaction with another instruction causes an exception
+Specific checks required:
+Sequential execution with word aligned 16-bit instruction.
+Sequential execution with non-word aligned 16-bit instruction.
+Word aligned 16-bit instruction reached via jump.
+Non-word aligned 16-bit instruction reached via jump.</t>
+  </si>
+  <si>
+    <t>Continous bus error</t>
+  </si>
+  <si>
+    <t>A faulty memory can cause non-stop data bus error. This will stop meaningful execution, but behaviour needs to be verified regardless</t>
+  </si>
+  <si>
+    <t>Verify behaviour during continous data bus error</t>
+  </si>
+  <si>
+    <t>Verify behaviour during continous instruction bus error</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The OBI agent will be required to randomly generate bus errors, and verify that the signals </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">instr_err_i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>data_err_i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve"> comply with the OBI Spec. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+In order to use randomization of bus errors without trigger errors with behaviour within spec when confronted with near-continous bus errors, the UVM agent will need to implement a minimum distance between bus errors. This should be controllable via parameter.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that a bus error results in a machine mode exception.
+Especially check that the exception is taken with local and global interrupts disabled</t>
+  </si>
+  <si>
+    <t>A bus error shall appear according to debug spec when in debug mode.</t>
+  </si>
+  <si>
+    <t>A bus error shall appear according to debug spec when in single step mode</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify a bus error in single step mode
+Verify that debug is reentered immediately after updating </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>pc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>tval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>cause</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify a bus error in debug mode
+Verify no registers are updated by the exception</t>
+  </si>
+  <si>
+    <t>RISC-V Zce code-size reduction extension proposal v0.41.5</t>
+  </si>
+  <si>
+    <t>RV_ZCE</t>
+  </si>
+  <si>
+    <t>https://github.com/riscv/riscv-code-size-reduction/blob/master/ISA%20proposals/Huawei/Zce_spec.adoc</t>
+  </si>
+  <si>
+    <t>UM 828dac, RV_ZCE</t>
+  </si>
+  <si>
+    <t>Instruction bus error with ZCE Table jump</t>
+  </si>
+  <si>
+    <t>ZCE tablejump proposal specifies exception handling</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">mepc </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">is set to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>pc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve"> of the C.TBLJ*, and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>mtval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve"> is set to the address in the jump table entry</t>
+    </r>
+  </si>
+  <si>
+    <t>verify correct operation for bus error with zce table jump</t>
   </si>
 </sst>
 </file>
@@ -635,7 +798,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -658,12 +821,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -691,38 +891,56 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1107,12 +1325,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ79"/>
+  <dimension ref="A1:AMJ86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -1130,7 +1348,7 @@
     <col min="1024" max="1024" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="30">
+    <row r="1" spans="1:9" s="5" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1160,559 +1378,626 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="19" t="s">
+      <c r="F3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A5" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A7" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A8" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A3" s="20" t="s">
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A9" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="143.25">
+      <c r="A10" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" s="5" customFormat="1" ht="186">
+      <c r="A11" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="86.25">
+      <c r="A17" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="E17" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A18" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A19" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A20" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A21" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" s="5" customFormat="1" ht="43.5">
+      <c r="A22" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A23" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="43.5" customHeight="1">
+      <c r="A24" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="21"/>
-    </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A4" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="21" t="s">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" ht="29.25">
+      <c r="A25" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A6" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" ht="44.25">
-      <c r="A8" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A9" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" ht="43.5" customHeight="1">
-      <c r="A11" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A12" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A13" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A14" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="21"/>
-    </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A15" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A16" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="43.5">
-      <c r="A18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="21"/>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="29.25">
-      <c r="A19" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:9" s="5" customFormat="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" s="5" customFormat="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" s="5" customFormat="1">
-      <c r="A22" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" s="5" customFormat="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" s="5" customFormat="1">
-      <c r="A24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="65.25" customHeight="1">
-      <c r="A26" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="27"/>
+    <row r="26" spans="1:9" s="5" customFormat="1">
+      <c r="A26" s="32"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="63" customHeight="1">
-      <c r="A27" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="22"/>
+    <row r="27" spans="1:9" s="5" customFormat="1">
+      <c r="A27" s="32"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1720,14 +2005,10 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" ht="123" customHeight="1">
-      <c r="A28" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="22"/>
+    <row r="28" spans="1:9" s="5" customFormat="1">
+      <c r="A28" s="32"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1736,14 +2017,16 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="6"/>
+      <c r="A29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1">
@@ -1759,7 +2042,6 @@
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1">
       <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1768,10 +2050,14 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" s="5" customFormat="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="A32" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="27"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1779,21 +2065,29 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" s="5" customFormat="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+    <row r="33" spans="1:9" s="5" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A33" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" s="5" customFormat="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+    <row r="34" spans="1:9" s="5" customFormat="1" ht="132.75" customHeight="1">
+      <c r="A34" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="25"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1801,10 +2095,14 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" s="5" customFormat="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+    <row r="35" spans="1:9" s="5" customFormat="1" ht="123" customHeight="1">
+      <c r="A35" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2285,30 +2583,113 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="1:9" s="8" customFormat="1">
-      <c r="A79" s="13" t="s">
+    <row r="79" spans="1:9" s="5" customFormat="1">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+    </row>
+    <row r="80" spans="1:9" s="5" customFormat="1">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="1:9" s="5" customFormat="1">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="1:9" s="5" customFormat="1">
+      <c r="A82" s="6"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="1:9" s="5" customFormat="1">
+      <c r="A83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="1:9" s="5" customFormat="1">
+      <c r="A84" s="6"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="1:9" s="5" customFormat="1">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="1:9" s="8" customFormat="1">
+      <c r="A86" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A79:I79"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+  <mergeCells count="15">
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2322,7 +2703,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H21 H23:H78</xm:sqref>
+          <xm:sqref>H30:H85 H2:H28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -2331,7 +2712,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G23:G78 G2:G21</xm:sqref>
+          <xm:sqref>G30:G85 G2:G28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -2340,7 +2721,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F23:F78 F2:F21</xm:sqref>
+          <xm:sqref>F30:F85 F2:F28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2463,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -2494,38 +2875,49 @@
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="12" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="12" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>